<commit_message>
- 更新luban版本到v2.6.0 - luban.conf中为editor新增单独的target配置
</commit_message>
<xml_diff>
--- a/DataTables/Datas/test/define_from_excel.xlsx
+++ b/DataTables/Datas/test/define_from_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace2\luban_examples\DataTables\Datas\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A7D75B-7197-4D01-B5CF-BFA3084D9643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA6D36E-31C9-46EC-8CF3-63BA868F19A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42300" yWindow="3600" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="109">
   <si>
     <t>##</t>
   </si>
@@ -367,6 +367,58 @@
   </si>
   <si>
     <t>1,2,3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{},2,3,4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>vec3,2,2,2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>c1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>array,array,int</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>c2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>list,list,int</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>c3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>list,set,int</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>c4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>map,int,list,int</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>c5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>map,int,map,int,int</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -470,6 +522,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -479,7 +532,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="差" xfId="2" builtinId="27"/>
@@ -757,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -781,9 +833,11 @@
     <col min="16" max="16" width="17.5" customWidth="1"/>
     <col min="20" max="20" width="33.625" customWidth="1"/>
     <col min="21" max="21" width="18.125" customWidth="1"/>
+    <col min="30" max="30" width="12.375" customWidth="1"/>
+    <col min="33" max="33" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,11 +862,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
@@ -828,32 +882,47 @@
       <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
       <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8" t="s">
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
       <c r="AB1" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -878,11 +947,11 @@
       <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
       <c r="L2" s="2" t="s">
         <v>27</v>
       </c>
@@ -898,32 +967,47 @@
       <c r="P2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
       <c r="T2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9" t="s">
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
       <c r="AB2" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="AD2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -940,7 +1024,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -952,7 +1036,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>10000</v>
       </c>
@@ -1023,7 +1107,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>10001</v>
       </c>
@@ -1093,11 +1177,11 @@
       <c r="AA6" t="s">
         <v>60</v>
       </c>
-      <c r="AB6" s="10" t="s">
+      <c r="AB6" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>10002</v>
       </c>
@@ -1164,8 +1248,11 @@
       <c r="AA7" t="s">
         <v>65</v>
       </c>
+      <c r="AB7" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>10003</v>
       </c>
@@ -1232,8 +1319,11 @@
       <c r="AA8" t="s">
         <v>70</v>
       </c>
+      <c r="AB8" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>10004</v>
       </c>
@@ -1300,8 +1390,11 @@
       <c r="AA9" t="s">
         <v>75</v>
       </c>
+      <c r="AB9" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>10005</v>
       </c>
@@ -1366,7 +1459,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>10006</v>
       </c>
@@ -1425,7 +1518,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>10007</v>
       </c>
@@ -1484,7 +1577,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>10008</v>
       </c>

</xml_diff>

<commit_message>
- 升级luban到v4.3.0 - 新增constalias示例
</commit_message>
<xml_diff>
--- a/DataTables/Datas/test/define_from_excel.xlsx
+++ b/DataTables/Datas/test/define_from_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace2\luban_examples\DataTables\Datas\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban\luban_examples\DataTables\Datas\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A1F0A0-87E7-4BC6-9805-0E9A4FA355C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2722BB60-2AE2-4F23-968F-3A05BA2D61F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35940" yWindow="4620" windowWidth="34200" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5895" yWindow="3465" windowWidth="30000" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>